<commit_message>
chore: clean data/ and main
</commit_message>
<xml_diff>
--- a/data/worldbank_venezuela_data.xls_clean.xlsx
+++ b/data/worldbank_venezuela_data.xls_clean.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Year</t>
+  </si>
   <si>
     <t>GDP (current LCU)</t>
   </si>
@@ -453,27 +456,29 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
add individual country excel data
</commit_message>
<xml_diff>
--- a/data/worldbank_venezuela_data.xls_clean.xlsx
+++ b/data/worldbank_venezuela_data.xls_clean.xlsx
@@ -61,7 +61,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -75,6 +75,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -97,35 +104,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -439,7 +439,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -455,7 +455,7 @@
     <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,32 +609,6 @@
       </c>
       <c r="H6" s="5">
         <v>2665390596.96136</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="2">
-        <v>2010</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1016834748000</v>
-      </c>
-      <c r="C7" s="5">
-        <v>13692.91496662106</v>
-      </c>
-      <c r="D7" s="5">
-        <v>31.43295512163202</v>
-      </c>
-      <c r="E7" s="5">
-        <v>28247997757.24063</v>
-      </c>
-      <c r="F7" s="5">
-        <v>93.39691133131616</v>
-      </c>
-      <c r="G7" s="4">
-        <v>12831302</v>
-      </c>
-      <c r="H7" s="5">
-        <v>3991194834.74435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>